<commit_message>
added support for sameAs URLs in context
</commit_message>
<xml_diff>
--- a/test_data/luckett/CATALOG.xlsx
+++ b/test_data/luckett/CATALOG.xlsx
@@ -618,8 +618,8 @@
         <v>IDEAL Nursing home facility descriptors N=20.sav</v>
       </c>
       <c r="C3" t="str" xml:space="preserve">
-        <v xml:space="preserve">Baseline characteristics of the 20 nursing homes (Table 1)._x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Baseline characteristics of the 20 nursing homes (Table 1)._x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
 N.B. Table 1 Questionnaire on Palliative care for Advanced Dementia (qPAD) median scores by group calculated using staff level data in Dataset 2.</v>
       </c>
       <c r="E3" t="str">
@@ -645,18 +645,18 @@
         <v>IDEAL Staff qPAD baseline scores N=290.sav</v>
       </c>
       <c r="C5" t="str" xml:space="preserve">
-        <v xml:space="preserve">Contains _x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d_
-baseline characteristics of the 131 residents (Table 1)_x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d_
-End of Life Outcomes (family-rated and nurse-rated) total scores and weeks to completion (Tables 2, 3 and 4)_x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d_
-N.B. there are more ‘time to completion’ data points than EOLD (End Of Life Dementia) scores since some EOLD responses were provided but unable to generate a valid total score._x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d_
-Case conference (whether or not resident received at least one case conference)_x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d_
-Quality of Life in Late-stage Dementia (QUALID) data_x000d__x000d__x000d__x000d_
-_x000d__x000d__x000d__x000d_
+        <v xml:space="preserve">Contains _x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
+baseline characteristics of the 131 residents (Table 1)_x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
+End of Life Outcomes (family-rated and nurse-rated) total scores and weeks to completion (Tables 2, 3 and 4)_x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
+N.B. there are more ‘time to completion’ data points than EOLD (End Of Life Dementia) scores since some EOLD responses were provided but unable to generate a valid total score._x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
+Case conference (whether or not resident received at least one case conference)_x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
+Quality of Life in Late-stage Dementia (QUALID) data_x000d__x000d__x000d__x000d__x000d_
+_x000d__x000d__x000d__x000d__x000d_
 Symptoms and care during the last month of life (Table 5)</v>
       </c>
       <c r="E5" t="str">
@@ -670,7 +670,7 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="People"/>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -697,9 +697,6 @@
       <c r="G1" t="str">
         <v>ID</v>
       </c>
-      <c r="J1" t="str">
-        <v>contactPoint&gt;TYPE:ContactPoint&gt;</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -741,9 +738,6 @@
       </c>
       <c r="G3" t="str">
         <v>http://orcid.org/0000-0001-6121-5409</v>
-      </c>
-      <c r="J3" t="str">
-        <v>ID: tim.luckett@uts.edu.au, contactType: customer service, email: tim.luckett@uts.edu.au, name: Contact Tim Luckett</v>
       </c>
     </row>
     <row r="4">
@@ -1017,7 +1011,7 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr codeName="Organisations"/>
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1041,6 +1035,9 @@
       <c r="F1" t="str">
         <v>TYPE:</v>
       </c>
+      <c r="G1" t="str">
+        <v>contactPoint&gt;TYPE:ContactPoint&gt;</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
@@ -1072,6 +1069,9 @@
       <c r="F3" t="str">
         <v>Organization</v>
       </c>
+      <c r="G3" t="str">
+        <v>ID: tim.luckett@uts.edu.au, contactType: customer service, email: tim.luckett@uts.edu.au, name: Contact Tim Luckett</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -1277,6 +1277,9 @@
       </c>
       <c r="F16" t="str">
         <v>Organization</v>
+      </c>
+      <c r="G16" t="str">
+        <v>ID: tim.luckett@uts.edu.au, contactType: customer service, email: tim.luckett@uts.edu.au, name: Contact Tim Luckett</v>
       </c>
     </row>
     <row r="17">

</xml_diff>